<commit_message>
TICKET-15991 PDB Upgrade (JAST Purchase_20220507.zip)
git-svn-id: svn+ssh://devteam/data/svn/tcijapp/Purchase/trunk@1958 ebf3080d-37d0-4b6c-8d7e-121e4dec3f32
</commit_message>
<xml_diff>
--- a/Purchase/App_Data/RFQList.xlsx
+++ b/Purchase/App_Data/RFQList.xlsx
@@ -4,12 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -362,56 +374,54 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1"/>

</xml_diff>